<commit_message>
so falta o dias
a
</commit_message>
<xml_diff>
--- a/relatorios/dias-salvos-2025-04.xlsx
+++ b/relatorios/dias-salvos-2025-04.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Data</t>
   </si>
@@ -26,6 +26,9 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>Média</t>
   </si>
 </sst>
 </file>
@@ -402,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C3"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -426,14 +429,22 @@
         <v>3</v>
       </c>
       <c r="B2">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="C2" t="s">
         <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Ok. mudamos muita coisa
Ele continua com as mesmas funcionalidades mas eu juntei todos os arquivos para otimizar e diminuir tantos. Ele continua com o problema de salvar. Mas agora está salvando ao 12h e as 18h. Só que não escreve novamente.
</commit_message>
<xml_diff>
--- a/relatorios/dias-salvos-2025-04.xlsx
+++ b/relatorios/dias-salvos-2025-04.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
   <si>
     <t>Data</t>
   </si>
@@ -26,6 +26,15 @@
   </si>
   <si>
     <t>-</t>
+  </si>
+  <si>
+    <t>2025-04-12</t>
+  </si>
+  <si>
+    <t>2025-04-13</t>
+  </si>
+  <si>
+    <t>2025-04-14</t>
   </si>
   <si>
     <t>Média</t>
@@ -405,7 +414,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C12"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -435,16 +444,55 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B3">
-        <v>29</v>
+      <c r="B9">
+        <v>24</v>
+      </c>
+      <c r="C9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>27</v>
+      </c>
+      <c r="C11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>26</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1" firstPageNumber="1" useFirstPageNumber="1" copies="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adicionado banco para powerbi
</commit_message>
<xml_diff>
--- a/relatorios/dias-salvos-2025-04.xlsx
+++ b/relatorios/dias-salvos-2025-04.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="25">
   <si>
     <t>Data</t>
   </si>
@@ -35,6 +35,54 @@
   </si>
   <si>
     <t>2025-04-14</t>
+  </si>
+  <si>
+    <t>2025-04-15</t>
+  </si>
+  <si>
+    <t>2025-04-16</t>
+  </si>
+  <si>
+    <t>2025-04-17</t>
+  </si>
+  <si>
+    <t>2025-04-18</t>
+  </si>
+  <si>
+    <t>2025-04-19</t>
+  </si>
+  <si>
+    <t>2025-04-20</t>
+  </si>
+  <si>
+    <t>2025-04-21</t>
+  </si>
+  <si>
+    <t>2025-04-22</t>
+  </si>
+  <si>
+    <t>2025-04-23</t>
+  </si>
+  <si>
+    <t>2025-04-24</t>
+  </si>
+  <si>
+    <t>2025-04-25</t>
+  </si>
+  <si>
+    <t>2025-04-26</t>
+  </si>
+  <si>
+    <t>2025-04-27</t>
+  </si>
+  <si>
+    <t>2025-04-28</t>
+  </si>
+  <si>
+    <t>2025-04-29</t>
+  </si>
+  <si>
+    <t>2025-04-30</t>
   </si>
   <si>
     <t>Média</t>
@@ -414,7 +462,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C28"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1"/>
@@ -483,12 +531,188 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
       <c r="B12">
-        <v>26</v>
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>40</v>
+      </c>
+      <c r="C13" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14">
+        <v>38</v>
+      </c>
+      <c r="C14" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15">
+        <v>48</v>
+      </c>
+      <c r="C15" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16">
+        <v>30</v>
+      </c>
+      <c r="C16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>14</v>
+      </c>
+      <c r="B18">
+        <v>37</v>
+      </c>
+      <c r="C18" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19">
+        <v>43</v>
+      </c>
+      <c r="C19" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>16</v>
+      </c>
+      <c r="B20">
+        <v>31</v>
+      </c>
+      <c r="C20" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21">
+        <v>35</v>
+      </c>
+      <c r="C21" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22">
+        <v>39</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>19</v>
+      </c>
+      <c r="B23">
+        <v>37</v>
+      </c>
+      <c r="C23" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>21</v>
+      </c>
+      <c r="B25">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>22</v>
+      </c>
+      <c r="B26">
+        <v>29</v>
+      </c>
+      <c r="C26" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27">
+        <v>25</v>
+      </c>
+      <c r="C27" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>24</v>
+      </c>
+      <c r="B28">
+        <v>34</v>
       </c>
     </row>
   </sheetData>

</xml_diff>